<commit_message>
Updated king (moving), PGN (saving)
</commit_message>
<xml_diff>
--- a/chessboard.xlsx
+++ b/chessboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\OneDrive\Desktop\Projects\Surchessake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87B3F436-0F63-4ED0-B5F1-F5CD3399D8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BF2310-5690-4E7E-A174-CD7CC79DC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
+    <workbookView xWindow="21100" yWindow="290" windowWidth="17280" windowHeight="8960" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -66,13 +95,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +513,7 @@
   <dimension ref="A1:AV28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1396,14 +1519,41 @@
       <c r="H11" s="1">
         <v>7</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AB11" s="1"/>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="5"/>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11" s="1">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>7</v>
+      </c>
+      <c r="X11" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y11">
+        <v>11</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA11">
+        <v>5</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>3</v>
+      </c>
       <c r="AF11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AJ11" s="1"/>
@@ -1458,14 +1608,41 @@
       <c r="H12">
         <v>15</v>
       </c>
-      <c r="K12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="AA12" s="1"/>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="U12" s="1">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
       <c r="AE12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AI12" s="1"/>
@@ -1520,14 +1697,41 @@
       <c r="H13" s="1">
         <v>23</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AB13" s="1"/>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="11"/>
+      <c r="U13">
+        <v>-1</v>
+      </c>
+      <c r="V13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="W13">
+        <v>-1</v>
+      </c>
+      <c r="X13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Y13">
+        <v>-1</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AA13">
+        <v>-1</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>-1</v>
+      </c>
       <c r="AF13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AJ13" s="1"/>
@@ -1582,14 +1786,41 @@
       <c r="H14">
         <v>31</v>
       </c>
-      <c r="K14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="AA14" s="1"/>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
+      <c r="U14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="V14">
+        <v>-1</v>
+      </c>
+      <c r="W14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="X14">
+        <v>-1</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Z14">
+        <v>-1</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AB14">
+        <v>-1</v>
+      </c>
       <c r="AE14" s="1"/>
       <c r="AG14" s="1"/>
       <c r="AI14" s="1"/>
@@ -1644,14 +1875,41 @@
       <c r="H15" s="1">
         <v>39</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AB15" s="1"/>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="11"/>
+      <c r="U15">
+        <v>-1</v>
+      </c>
+      <c r="V15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="W15">
+        <v>-1</v>
+      </c>
+      <c r="X15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Y15">
+        <v>-1</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AA15">
+        <v>-1</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>-1</v>
+      </c>
       <c r="AF15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AJ15" s="1"/>
@@ -1706,14 +1964,41 @@
       <c r="H16">
         <v>47</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="AA16" s="1"/>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="9"/>
+      <c r="U16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="V16">
+        <v>-1</v>
+      </c>
+      <c r="W16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="X16">
+        <v>-1</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Z16">
+        <v>-1</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AB16">
+        <v>-1</v>
+      </c>
       <c r="AE16" s="1"/>
       <c r="AG16" s="1"/>
       <c r="AI16" s="1"/>
@@ -1768,14 +2053,41 @@
       <c r="H17" s="1">
         <v>55</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AB17" s="1"/>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="11"/>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
       <c r="AF17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AJ17" s="1"/>
@@ -1830,14 +2142,41 @@
       <c r="H18">
         <v>63</v>
       </c>
-      <c r="K18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="15"/>
+      <c r="U18" s="1">
+        <v>2</v>
+      </c>
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18" s="1">
+        <v>6</v>
+      </c>
+      <c r="X18">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z18">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB18">
+        <v>2</v>
+      </c>
       <c r="AE18" s="1"/>
       <c r="AG18" s="1"/>
       <c r="AI18" s="1"/>
@@ -1867,6 +2206,32 @@
         <v>63</v>
       </c>
     </row>
+    <row r="19" spans="1:48" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="21" spans="1:48" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>

</xml_diff>

<commit_message>
Bishop movement, Rook movement, Queen movement, and Pawn capture fix
</commit_message>
<xml_diff>
--- a/chessboard.xlsx
+++ b/chessboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\OneDrive\Desktop\Projects\Surchessake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BF2310-5690-4E7E-A174-CD7CC79DC964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C9E51-6D41-45D8-8D56-0012D2B4B235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21100" yWindow="290" windowWidth="17280" windowHeight="8960" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
+    <workbookView xWindow="4836" yWindow="2208" windowWidth="13380" windowHeight="10152" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +83,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -196,6 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35CD89D-339A-4853-84D9-B5DF3BC73661}">
   <dimension ref="A1:AV28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1516,7 +1523,7 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="16">
         <v>7</v>
       </c>
       <c r="J11">
@@ -1605,7 +1612,7 @@
       <c r="G12" s="1">
         <v>14</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="16">
         <v>15</v>
       </c>
       <c r="J12">
@@ -1694,7 +1701,7 @@
       <c r="G13">
         <v>22</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="16">
         <v>23</v>
       </c>
       <c r="J13">
@@ -1783,7 +1790,7 @@
       <c r="G14" s="1">
         <v>30</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="16">
         <v>31</v>
       </c>
       <c r="J14">
@@ -1872,7 +1879,7 @@
       <c r="G15">
         <v>38</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="16">
         <v>39</v>
       </c>
       <c r="J15">
@@ -1961,7 +1968,7 @@
       <c r="G16" s="1">
         <v>46</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="16">
         <v>47</v>
       </c>
       <c r="J16">
@@ -2050,7 +2057,7 @@
       <c r="G17">
         <v>54</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="16">
         <v>55</v>
       </c>
       <c r="J17">
@@ -2139,7 +2146,7 @@
       <c r="G18" s="1">
         <v>62</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="16">
         <v>63</v>
       </c>
       <c r="J18">
@@ -2231,6 +2238,7 @@
       <c r="R19" t="s">
         <v>6</v>
       </c>
+      <c r="V19" s="16"/>
     </row>
     <row r="21" spans="1:48" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">

</xml_diff>

<commit_message>
New Beta + UI Improvements!
</commit_message>
<xml_diff>
--- a/chessboard.xlsx
+++ b/chessboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\OneDrive\Desktop\Projects\Surchessake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C9E51-6D41-45D8-8D56-0012D2B4B235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F1ED6-0428-4E40-983C-B62659A5E843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4836" yWindow="2208" windowWidth="13380" windowHeight="10152" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38A1CE69-53A4-45C2-AE53-31C8A2F7FD44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>a</t>
   </si>
@@ -59,12 +59,15 @@
   <si>
     <t>g</t>
   </si>
+  <si>
+    <t>NG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,8 +75,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,8 +102,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -181,11 +209,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -203,6 +272,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35CD89D-339A-4853-84D9-B5DF3BC73661}">
-  <dimension ref="A1:AV28"/>
+  <dimension ref="A1:AV42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF14" sqref="AF14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="AL36" activeCellId="4" sqref="AJ32 AK33 AL34 AM35 AL36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3216,7 +3299,170 @@
         <v>63</v>
       </c>
     </row>
+    <row r="33" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S33" s="2"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="17"/>
+    </row>
+    <row r="34" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S34" s="10"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD34" s="30"/>
+      <c r="AE34" s="20"/>
+      <c r="AF34" s="9"/>
+    </row>
+    <row r="35" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S35" s="10"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="9"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="21"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="23"/>
+      <c r="AF35" s="9"/>
+    </row>
+    <row r="36" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="25"/>
+      <c r="AE36" s="26"/>
+      <c r="AF36" s="9"/>
+    </row>
+    <row r="37" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S37" s="10"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="9"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="24"/>
+      <c r="AD37" s="25"/>
+      <c r="AE37" s="26"/>
+      <c r="AF37" s="9"/>
+    </row>
+    <row r="38" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="24"/>
+      <c r="AD38" s="25"/>
+      <c r="AE38" s="26"/>
+      <c r="AF38" s="9"/>
+    </row>
+    <row r="39" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S39" s="10"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="9"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="24"/>
+      <c r="AD39" s="25"/>
+      <c r="AE39" s="26"/>
+      <c r="AF39" s="9"/>
+    </row>
+    <row r="40" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="7"/>
+      <c r="AC40" s="27"/>
+      <c r="AD40" s="28"/>
+      <c r="AE40" s="29"/>
+      <c r="AF40" s="9"/>
+    </row>
+    <row r="41" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S41" s="10"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="14"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="7"/>
+      <c r="AC41" s="19"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="9"/>
+    </row>
+    <row r="42" spans="19:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S42" s="18"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="13"/>
+      <c r="AF42" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>